<commit_message>
Fix typo in main.blade.php
</commit_message>
<xml_diff>
--- a/public/pdf_file/Laporan_Keuangan.xlsx
+++ b/public/pdf_file/Laporan_Keuangan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Pendataan-Desa\public\pdf_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3284FC7-3B33-4062-A721-84398B38A271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC9A0D-7BDB-4041-9465-CF5C91174FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{434B3040-041E-43FD-AB34-AECA2D945A56}"/>
   </bookViews>
@@ -566,86 +566,86 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -967,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -987,28 +987,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="49">
         <v>45399</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1031,11 +1031,11 @@
       <c r="G4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -1049,11 +1049,11 @@
       <c r="G5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -1067,11 +1067,11 @@
       <c r="G6" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -1080,12 +1080,12 @@
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1095,19 +1095,19 @@
       <c r="D9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="27"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="14" t="s">
         <v>77</v>
       </c>
@@ -1115,21 +1115,21 @@
         <v>100</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="33">
+      <c r="I10" s="36">
         <v>0.05</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="14" t="s">
         <v>78</v>
       </c>
@@ -1137,21 +1137,21 @@
         <v>61</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="33"/>
+      <c r="J11" s="36"/>
     </row>
     <row r="12" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="25" t="s">
         <v>80</v>
       </c>
@@ -1163,11 +1163,11 @@
         <v>11</v>
       </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="34" t="s">
+      <c r="H12" s="28"/>
+      <c r="I12" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="34"/>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -1181,22 +1181,22 @@
         <v>100</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="42" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="37"/>
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="24" t="s">
         <v>79</v>
       </c>
@@ -1208,21 +1208,21 @@
         <v>7</v>
       </c>
       <c r="G14" s="47"/>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="37"/>
+      <c r="J14" s="44"/>
       <c r="O14" s="5"/>
       <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="14" t="s">
         <v>81</v>
       </c>
@@ -1230,25 +1230,25 @@
         <v>63</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="51" t="s">
+      <c r="G15" s="32"/>
+      <c r="H15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="37" t="s">
+      <c r="I15" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="37"/>
+      <c r="J15" s="44"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="24" t="s">
         <v>82</v>
       </c>
@@ -1256,23 +1256,23 @@
         <v>64</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="46"/>
-      <c r="H16" s="51" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="40"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="24" t="s">
         <v>83</v>
       </c>
@@ -1280,23 +1280,23 @@
         <v>65</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="32"/>
+      <c r="H17" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="38"/>
+      <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="14" t="s">
         <v>84</v>
       </c>
@@ -1304,23 +1304,23 @@
         <v>66</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="51" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="38"/>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="14" t="s">
         <v>85</v>
       </c>
@@ -1328,23 +1328,23 @@
         <v>67</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="51" t="s">
+      <c r="G19" s="32"/>
+      <c r="H19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="I19" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="38"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="14" t="s">
         <v>86</v>
       </c>
@@ -1352,45 +1352,45 @@
         <v>68</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="35">
+      <c r="G20" s="32"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="45">
         <v>0.05</v>
       </c>
-      <c r="J20" s="35"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="52" t="s">
+      <c r="B21" s="39"/>
+      <c r="C21" s="31" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>69</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="51" t="s">
+      <c r="G21" s="32"/>
+      <c r="H21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="36"/>
+      <c r="J21" s="46"/>
     </row>
     <row r="22" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="40"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="24" t="s">
         <v>88</v>
       </c>
@@ -1398,19 +1398,19 @@
         <v>70</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
     </row>
     <row r="23" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="24" t="s">
         <v>89</v>
       </c>
@@ -1421,18 +1421,18 @@
       <c r="F23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="24" t="s">
         <v>94</v>
       </c>
@@ -1440,17 +1440,17 @@
         <v>72</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="24" t="s">
         <v>90</v>
       </c>
@@ -1461,18 +1461,18 @@
       <c r="F25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="40"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="24" t="s">
         <v>91</v>
       </c>
@@ -1483,18 +1483,18 @@
       <c r="F26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="40"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="24" t="s">
         <v>92</v>
       </c>
@@ -1504,18 +1504,18 @@
       <c r="F27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="27"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="14" t="s">
         <v>93</v>
       </c>
@@ -1524,17 +1524,54 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="G23:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="G27:J27"/>
@@ -1545,49 +1582,12 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="F22:J22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="G23:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix PDF link and update financial information in main.blade.php
</commit_message>
<xml_diff>
--- a/public/pdf_file/Laporan_Keuangan.xlsx
+++ b/public/pdf_file/Laporan_Keuangan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Pendataan-Desa\public\pdf_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC9A0D-7BDB-4041-9465-CF5C91174FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A115952-DB37-4D0C-8605-42B803F32571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{434B3040-041E-43FD-AB34-AECA2D945A56}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
   <si>
     <t>Finansial</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Growth rate</t>
-  </si>
-  <si>
-    <t>Operating Long Term Asset dengan asumsi harga tanah Rp 100.000 / m²</t>
   </si>
   <si>
     <t>WACC</t>
@@ -344,6 +341,21 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>Operating Long Term Asset dengan asumsi harga tanah Rp 100.000 /m²</t>
+  </si>
+  <si>
+    <t>Komoditi Panen</t>
+  </si>
+  <si>
+    <t>Periode Tanam</t>
+  </si>
+  <si>
+    <t>Beras Cianjur</t>
+  </si>
+  <si>
+    <t>1 Maret - 30 Juni 2024</t>
+  </si>
 </sst>
 </file>
 
@@ -352,7 +364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,13 +479,6 @@
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -499,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -537,9 +542,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -584,6 +586,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -602,8 +610,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -621,31 +638,22 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -965,16 +973,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.21875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" style="8" customWidth="1"/>
@@ -986,32 +994,32 @@
     <col min="11" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="16" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="49">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="51">
         <v>45399</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="G3" s="15"/>
@@ -1019,578 +1027,628 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>99</v>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="G4" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-    </row>
-    <row r="5" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>101</v>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="G5" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-    </row>
-    <row r="6" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="G6" s="20" t="s">
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-    </row>
-    <row r="10" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="14" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="14">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="14">
         <v>100</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="36">
+      <c r="E21" s="3"/>
+      <c r="F21" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="26"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="38"/>
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="48"/>
+      <c r="H22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="42"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="43"/>
+      <c r="C23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="33"/>
+      <c r="H23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="42"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="38"/>
+    </row>
+    <row r="25" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="38"/>
+    </row>
+    <row r="26" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="43"/>
+      <c r="C26" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="H26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="38"/>
+    </row>
+    <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="43"/>
+      <c r="C27" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="38"/>
+    </row>
+    <row r="28" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="33"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="40">
         <v>0.05</v>
       </c>
-      <c r="J10" s="36"/>
-    </row>
-    <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="J11" s="36"/>
-    </row>
-    <row r="12" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" s="48"/>
-    </row>
-    <row r="13" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="14" t="s">
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="33"/>
+      <c r="H29" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29" s="41"/>
+    </row>
+    <row r="30" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="43"/>
+      <c r="C30" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+    </row>
+    <row r="31" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="43"/>
+      <c r="C31" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+    </row>
+    <row r="32" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+    </row>
+    <row r="33" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="43"/>
+      <c r="C34" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+    </row>
+    <row r="35" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="43"/>
+      <c r="C35" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+    </row>
+    <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="14">
-        <v>100</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="43" t="s">
+      <c r="F36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+    </row>
+    <row r="37" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="45"/>
+      <c r="C37" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="37"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="44"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="44"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="37"/>
-    </row>
-    <row r="18" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="45">
-        <v>0.05</v>
-      </c>
-      <c r="J20" s="45"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="46"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-    </row>
-    <row r="24" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-    </row>
-    <row r="26" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="52"/>
+      <c r="D37" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="G23:J24"/>
-    <mergeCell ref="G25:J25"/>
+  <mergeCells count="50">
+    <mergeCell ref="G32:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H2:J2"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F19:G19"/>
     <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I23:J23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.3" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>